<commit_message>
Upload Non-Linear Fit + plot on the LP practice
</commit_message>
<xml_diff>
--- a/LO6/LP/data.xlsx
+++ b/LO6/LP/data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LO6/LP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3D3ABF-E76A-DD4D-A402-B1A8C1BE3E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D285E216-8939-1E43-AE2E-7D4FC419403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{2B7DD4B2-E682-AE46-809C-5F1CDB239214}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" activeTab="1" xr2:uid="{2B7DD4B2-E682-AE46-809C-5F1CDB239214}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>P1</t>
   </si>
@@ -99,6 +100,24 @@
   </si>
   <si>
     <t>R^2/A^2</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>dr</t>
+  </si>
+  <si>
+    <t>d(R^2/A^2)</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -656,48 +675,48 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$17:$H$29</c:f>
+              <c:f>Sheet1!$I$17:$I$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.1195126775048454E-3</c:v>
+                  <c:v>3.3459119496855344E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4350171291039496E-3</c:v>
+                  <c:v>3.7881619937694712E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8506229975080108E-3</c:v>
+                  <c:v>4.301886792452831E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5671111111111116E-3</c:v>
+                  <c:v>5.0666666666666672E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5698746093904515E-3</c:v>
+                  <c:v>5.9748427672955975E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8036232743957916E-3</c:v>
+                  <c:v>6.9308176100628935E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.2647742160887431E-3</c:v>
+                  <c:v>8.5233644859813093E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1861313457749829E-2</c:v>
+                  <c:v>0.10890965732087228</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9512869634417371E-2</c:v>
+                  <c:v>0.13968847352024924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0695913277239167E-2</c:v>
+                  <c:v>0.17520249221183803</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2742485030230685E-2</c:v>
+                  <c:v>0.22965732087227414</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.7670853349637501E-2</c:v>
+                  <c:v>0.31252336448598128</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.18161935540221857</c:v>
+                  <c:v>0.42616822429906548</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2012,16 +2031,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2048,16 +2067,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2384,8 +2403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5AB616-5E1C-C940-9C69-E68C1BE3BB78}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2472,11 +2491,11 @@
         <v>0.1</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G10" si="0">E4/D4</f>
+        <f t="shared" ref="G4:G6" si="0">E4/D4</f>
         <v>1.276595744680851E-2</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H10" si="1">G4*SQRT((F4/E4)^2 + (F4/D4)^2)</f>
+        <f t="shared" ref="H4:H6" si="1">G4*SQRT((F4/E4)^2 + (F4/D4)^2)</f>
         <v>1.0639164696969662E-2</v>
       </c>
     </row>
@@ -2507,6 +2526,22 @@
         <f t="shared" si="1"/>
         <v>1.100558617564492E-2</v>
       </c>
+      <c r="J5">
+        <f>G6/G3</f>
+        <v>0.64889261579440649</v>
+      </c>
+      <c r="K5">
+        <f>J5*SQRT((H6/G6)^2 + (H3/G3)^2)</f>
+        <v>9.8766935708425544E-3</v>
+      </c>
+      <c r="M5">
+        <f>G5/G3</f>
+        <v>3.943424996056575E-3</v>
+      </c>
+      <c r="N5">
+        <f>M5*SQRT((H5/G5)^2 + (H3/G3)^2)</f>
+        <v>7.9109519610351311E-4</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2613,6 +2648,22 @@
         <f>G10*SQRT((F10/E10)^2 + (F10/D10)^2)</f>
         <v>8.8864447334127947E-2</v>
       </c>
+      <c r="J10">
+        <f>G10/G8</f>
+        <v>0.66508012820512818</v>
+      </c>
+      <c r="K10">
+        <f>J10*SQRT((H10/G10)^2 + (H8/G8)^2)</f>
+        <v>9.7542112085360726E-3</v>
+      </c>
+      <c r="M10">
+        <f>G9/G8</f>
+        <v>4.3876026885735619E-3</v>
+      </c>
+      <c r="N10">
+        <f>M10*SQRT((H9/G9)^2 + (H8/G8)^2)</f>
+        <v>7.340008565264258E-4</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
@@ -2662,13 +2713,16 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>20</v>
       </c>
@@ -2680,17 +2734,32 @@
       </c>
       <c r="E17">
         <v>1.4</v>
+      </c>
+      <c r="F17">
+        <v>0.1</v>
       </c>
       <c r="G17">
         <f>E17/D17</f>
         <v>0.13207547169811321</v>
       </c>
       <c r="H17">
-        <f>(G17/$G$31)^2</f>
-        <v>1.1195126775048454E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ref="H11:H31" si="2">G17*SQRT((F17/E17)^2 + (F17/D17)^2)</f>
+        <v>9.5158892165351817E-3</v>
+      </c>
+      <c r="I17">
+        <f>G17/$G$31</f>
+        <v>3.3459119496855344E-2</v>
+      </c>
+      <c r="J17">
+        <f>I17*SQRT((H17/G17)^2 + ($H$31/$G$31)^2)</f>
+        <v>2.4296310270799371E-3</v>
+      </c>
+      <c r="K17">
+        <f>J17/I17</f>
+        <v>7.2614912275509397E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>25</v>
       </c>
@@ -2703,16 +2772,31 @@
       <c r="E18">
         <v>1.6</v>
       </c>
+      <c r="F18">
+        <v>0.1</v>
+      </c>
       <c r="G18">
-        <f t="shared" ref="G18:G29" si="2">E18/D18</f>
+        <f t="shared" ref="G18:G29" si="3">E18/D18</f>
         <v>0.14953271028037385</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:H29" si="3">(G18/$G$31)^2</f>
-        <v>1.4350171291039496E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>9.4497028826393721E-3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ref="I18:I29" si="4">G18/$G$31</f>
+        <v>3.7881619937694712E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18:J29" si="5">I18*SQRT((H18/G18)^2 + ($H$31/$G$31)^2)</f>
+        <v>2.4183428265854815E-3</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18:K29" si="6">J18/I18</f>
+        <v>6.3839477576804221E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>30</v>
       </c>
@@ -2725,16 +2809,31 @@
       <c r="E19">
         <v>1.8</v>
       </c>
+      <c r="F19">
+        <v>0.1</v>
+      </c>
       <c r="G19">
+        <f t="shared" si="3"/>
+        <v>0.169811320754717</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="2"/>
-        <v>0.169811320754717</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="3"/>
-        <v>1.8506229975080108E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9.5690139236138238E-3</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>4.301886792452831E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>2.4552072157734682E-3</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="6"/>
+        <v>5.7072799314032363E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>35</v>
       </c>
@@ -2747,16 +2846,31 @@
       <c r="E20">
         <v>2.1</v>
       </c>
+      <c r="F20">
+        <v>0.1</v>
+      </c>
       <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="3"/>
-        <v>2.5671111111111116E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9.7124181211291141E-3</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>5.0666666666666672E-2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>2.5028316227759294E-3</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="6"/>
+        <v>4.9397992554788078E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>40</v>
       </c>
@@ -2769,16 +2883,31 @@
       <c r="E21">
         <v>2.5</v>
       </c>
+      <c r="F21">
+        <v>0.1</v>
+      </c>
       <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.23584905660377359</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="2"/>
-        <v>0.23584905660377359</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="3"/>
-        <v>3.5698746093904515E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9.6927926521029849E-3</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>5.9748427672955975E-2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>2.5143261948423856E-3</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
+        <v>4.208188052420414E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>45</v>
       </c>
@@ -2791,16 +2920,31 @@
       <c r="E22">
         <v>2.9</v>
       </c>
+      <c r="F22">
+        <v>0.1</v>
+      </c>
       <c r="G22">
+        <f t="shared" si="3"/>
+        <v>0.27358490566037735</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="2"/>
-        <v>0.27358490566037735</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="3"/>
-        <v>4.8036232743957916E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9.7806519061489818E-3</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>6.9308176100628935E-2</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>2.5559078515558506E-3</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="6"/>
+        <v>3.6877436333700567E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>50</v>
       </c>
@@ -2813,16 +2957,31 @@
       <c r="E23">
         <v>3.6</v>
       </c>
+      <c r="F23">
+        <v>0.1</v>
+      </c>
       <c r="G23">
+        <f t="shared" si="3"/>
+        <v>0.33644859813084116</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="2"/>
-        <v>0.33644859813084116</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="3"/>
-        <v>7.2647742160887431E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9.8605778114397094E-3</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>8.5233644859813093E-2</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>2.6143728483393512E-3</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="6"/>
+        <v>3.0673014777665632E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>55</v>
       </c>
@@ -2835,16 +2994,31 @@
       <c r="E24">
         <v>4.5999999999999996</v>
       </c>
+      <c r="F24">
+        <v>0.1</v>
+      </c>
       <c r="G24">
+        <f t="shared" si="3"/>
+        <v>0.42990654205607476</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="2"/>
-        <v>0.42990654205607476</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="3"/>
-        <v>1.1861313457749829E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.0172843039890413E-2</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>0.10890965732087228</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>2.759132591468069E-3</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>2.5334140785504868E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>60</v>
       </c>
@@ -2857,16 +3031,31 @@
       <c r="E25">
         <v>5.9</v>
       </c>
+      <c r="F25">
+        <v>0.1</v>
+      </c>
       <c r="G25">
+        <f t="shared" si="3"/>
+        <v>0.55140186915887857</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="2"/>
-        <v>0.55140186915887857</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="3"/>
-        <v>1.9512869634417371E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.0672406249702808E-2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>0.13968847352024924</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>2.9845731807997744E-3</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="6"/>
+        <v>2.136592308288866E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>65</v>
       </c>
@@ -2879,16 +3068,31 @@
       <c r="E26">
         <v>7.4</v>
       </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
       <c r="G26">
+        <f t="shared" si="3"/>
+        <v>0.69158878504672905</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="2"/>
-        <v>0.69158878504672905</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="3"/>
-        <v>3.0695913277239167E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.1363098813221844E-2</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>0.17520249221183803</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>3.2863613945289375E-3</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="6"/>
+        <v>1.8757503692101506E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>70</v>
       </c>
@@ -2901,16 +3105,31 @@
       <c r="E27">
         <v>9.6999999999999993</v>
       </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
       <c r="G27">
+        <f t="shared" si="3"/>
+        <v>0.90654205607476634</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="2"/>
-        <v>0.90654205607476634</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="3"/>
-        <v>5.2742485030230685E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.2614463259642593E-2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>0.22965732087227414</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>3.8119664534197657E-3</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="6"/>
+        <v>1.6598497443675322E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>75</v>
       </c>
@@ -2923,16 +3142,31 @@
       <c r="E28">
         <v>13.2</v>
       </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
       <c r="G28">
+        <f t="shared" si="3"/>
+        <v>1.233644859813084</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="2"/>
-        <v>1.233644859813084</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="3"/>
-        <v>9.7670853349637501E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.4841520628779315E-2</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>0.31252336448598128</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>4.7047068420092483E-3</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>1.5053936366476962E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>80</v>
       </c>
@@ -2945,16 +3179,31 @@
       <c r="E29">
         <v>18</v>
       </c>
+      <c r="F29">
+        <v>0.1</v>
+      </c>
       <c r="G29">
+        <f t="shared" si="3"/>
+        <v>1.6822429906542058</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="2"/>
-        <v>1.6822429906542058</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="3"/>
-        <v>0.18161935540221857</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.828994044634152E-2</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
+        <v>0.42616822429906548</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>6.0283313528583593E-3</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="6"/>
+        <v>1.4145426639382551E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2963,14 +3212,232 @@
       </c>
       <c r="E31">
         <v>45</v>
+      </c>
+      <c r="F31">
+        <v>0.1</v>
       </c>
       <c r="G31">
         <f>E31/D31</f>
         <v>3.9473684210526314</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>3.5719872823425113E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6985BAE3-117D-9C4C-A8CB-7B098AEB4E05}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>3.3459119496855344E-2</v>
+      </c>
+      <c r="D2">
+        <v>2.4296310270799371E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>3.7881619937694712E-2</v>
+      </c>
+      <c r="D3">
+        <v>2.4183428265854815E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4">
+        <v>4.301886792452831E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.4552072157734682E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>5.0666666666666672E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.5028316227759294E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0.1</v>
+      </c>
+      <c r="C6">
+        <v>5.9748427672955975E-2</v>
+      </c>
+      <c r="D6">
+        <v>2.5143261948423856E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+      <c r="C7">
+        <v>6.9308176100628935E-2</v>
+      </c>
+      <c r="D7">
+        <v>2.5559078515558506E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+      <c r="C8">
+        <v>8.5233644859813093E-2</v>
+      </c>
+      <c r="D8">
+        <v>2.6143728483393512E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+      <c r="C9">
+        <v>0.10890965732087228</v>
+      </c>
+      <c r="D9">
+        <v>2.759132591468069E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>0.1</v>
+      </c>
+      <c r="C10">
+        <v>0.13968847352024924</v>
+      </c>
+      <c r="D10">
+        <v>2.9845731807997744E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>0.1</v>
+      </c>
+      <c r="C11">
+        <v>0.17520249221183803</v>
+      </c>
+      <c r="D11">
+        <v>3.2863613945289375E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>70</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+      <c r="C12">
+        <v>0.22965732087227414</v>
+      </c>
+      <c r="D12">
+        <v>3.8119664534197657E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>75</v>
+      </c>
+      <c r="B13">
+        <v>0.1</v>
+      </c>
+      <c r="C13">
+        <v>0.31252336448598128</v>
+      </c>
+      <c r="D13">
+        <v>4.7047068420092483E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>80</v>
+      </c>
+      <c r="B14">
+        <v>0.1</v>
+      </c>
+      <c r="C14">
+        <v>0.42616822429906548</v>
+      </c>
+      <c r="D14">
+        <v>6.0283313528583593E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update datasheet. Brewster uncertainty corrected. Upload VT guide.
</commit_message>
<xml_diff>
--- a/LO6/LP/data.xlsx
+++ b/LO6/LP/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LO6/LP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC293F1-9C86-4447-9E11-4686A060486D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE979453-A571-D24B-8C99-8087CD100E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{2B7DD4B2-E682-AE46-809C-5F1CDB239214}"/>
   </bookViews>
@@ -2406,13 +2406,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5AB616-5E1C-C940-9C69-E68C1BE3BB78}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -2574,6 +2575,12 @@
         <v>9.3777022415533581E-2</v>
       </c>
     </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f>B6-B5</f>
+        <v>-89</v>
+      </c>
+    </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>11</v>
@@ -2668,6 +2675,28 @@
         <v>7.340008565264258E-4</v>
       </c>
     </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f>B10-B9</f>
+        <v>-96</v>
+      </c>
+      <c r="J11">
+        <f>AVERAGE(J10,J5)</f>
+        <v>0.65698637199976728</v>
+      </c>
+      <c r="K11">
+        <f>_xlfn.T.INV.2T(0.05,1)*_xlfn.STDEV.S(J5,J10)/SQRT(2)</f>
+        <v>0.1028409234299994</v>
+      </c>
+      <c r="M11">
+        <f>AVERAGE(M10,M5)</f>
+        <v>4.1655138423150684E-3</v>
+      </c>
+      <c r="N11">
+        <f>_xlfn.T.INV.2T(0.05,1)*_xlfn.STDEV.S(M5,M10)/SQRT(2)</f>
+        <v>2.8219063501812459E-3</v>
+      </c>
+    </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>16</v>
@@ -2681,8 +2710,8 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <f>56.7*PI()/180</f>
-        <v>0.98960168588078479</v>
+        <f>57*PI()/180</f>
+        <v>0.99483767363676778</v>
       </c>
       <c r="C13">
         <f>0.5*PI()/180</f>
@@ -2690,11 +2719,11 @@
       </c>
       <c r="D13">
         <f>TAN(B13)</f>
-        <v>1.5223545068961311</v>
+        <v>1.5398649638145827</v>
       </c>
       <c r="E13">
-        <f>C13*1/(1+B13^2)</f>
-        <v>4.408930213627078E-3</v>
+        <f>C13/COS(B13)^2</f>
+        <v>2.9419131177139707E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>